<commit_message>
Update example templates and tests for template_reader
</commit_message>
<xml_diff>
--- a/tests/data/pbmc_invalid.xlsx
+++ b/tests/data/pbmc_invalid.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/manifests/pbmc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0A14F4-B6AC-B84F-B764-E7F5E00A48C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2709BEF-714C-9643-945A-66A47948D3D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24020" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41040" yWindow="2320" windowWidth="22600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CORE_DATA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -56,15 +56,28 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assigns a request identifier (mandatory or optional) for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assigns a request identifier (mandatory or optional) for the assay.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+          <t>Priority of the assay as it appears on the intake form.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -73,11 +86,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Priority of the assay as it appears on the intake form.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+          <t>Assay and sample type used. Example: Green-top tube - Plasma (Olink).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -86,11 +99,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assay and sample type used. Example: Green-top tube - Plasma (Olink).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+          <t>The number corresponding to the batch sent for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -99,11 +112,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The number corresponding to the batch sent for this assay.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+          <t>Box identifier for samples, if sample shipment container includes multiple boxes for each sample/assay type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -112,11 +125,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Box identifier for samples, if sample shipment container includes multiple boxes for each sample/assay type.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+          <t>Assay run number for samples received.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -125,11 +138,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assay run number for samples received.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+          <t>Courier utilized for shipment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -138,11 +151,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier utilized for shipment.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+          <t>Air bill number assigned to shipment. Example: 4567788343.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -151,11 +164,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Air bill number assigned to shipment. Example: 4567788343.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -164,11 +177,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+          <t>Type of shippment made.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -177,11 +190,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shippment made.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+          <t>Date of shipment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -190,11 +203,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of shipment.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+          <t>Count of specimens distributed by site.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -203,11 +216,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Count of specimens distributed by site.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+          <t>Number of Samples Received in Good Condition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -216,11 +229,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of Samples Received in Good Condition.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+          <t>Number if pathology report received.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -229,11 +242,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number if pathology report received.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+          <t>Shipping from [free text: person or organization, address, phone number, email address.]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -242,11 +255,63 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Shipping from [free text: person or organization, address, phone number, email address.]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+          <t>Shipping to [free text: person or organization, address, phone number, email address.]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Receiving site indicates how much material remains after assay use.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -255,11 +320,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Shipping to [free text: person or organization, address, phone number, email address.]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+          <t>Final status of sample after QC and pathology review.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status of sample if replacement is/was requested.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -272,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -285,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -298,7 +389,124 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -307,11 +515,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+          <t>Sample location within the shipping container. Example: A1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of sample sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -320,11 +541,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+          <t>The format in which the sample was sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quantity of each sample shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -333,11 +567,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+          <t>Volume of sample shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Volume units. Example: ml.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -346,24 +593,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -372,241 +606,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Time of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Time of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Type of sample sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The format in which the sample was sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Quantity of each sample shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Volume of sample shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Volume units. Example: ml.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample if replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -626,58 +626,58 @@
     <t>#p</t>
   </si>
   <si>
-    <t>LEAD_ORGANIZATION_STUDY_ID</t>
-  </si>
-  <si>
-    <t>MANIFEST_ID</t>
+    <t>LEAD ORGANIZATION STUDY ID</t>
+  </si>
+  <si>
+    <t>MANIFEST ID</t>
   </si>
   <si>
     <t>REQUEST</t>
   </si>
   <si>
-    <t>ASSAY_PRIORITY</t>
-  </si>
-  <si>
-    <t>ASSAY_TYPE</t>
-  </si>
-  <si>
-    <t>BATCH_NUMBER</t>
-  </si>
-  <si>
-    <t>BOX_NUMBER</t>
-  </si>
-  <si>
-    <t>ASSAY_RUN_NUMBER</t>
+    <t>ASSAY PRIORITY</t>
+  </si>
+  <si>
+    <t>ASSAY TYPE</t>
+  </si>
+  <si>
+    <t>BATCH NUMBER</t>
+  </si>
+  <si>
+    <t>BOX NUMBER</t>
+  </si>
+  <si>
+    <t>ASSAY RUN NUMBER</t>
   </si>
   <si>
     <t>COURIER</t>
   </si>
   <si>
-    <t>TRACKING_NUMBER</t>
-  </si>
-  <si>
-    <t>ACCOUNT_NUMBER</t>
-  </si>
-  <si>
-    <t>SHIPPING_CONDITION</t>
-  </si>
-  <si>
-    <t>DATE_SHIPPED</t>
-  </si>
-  <si>
-    <t>NUM_OF_SAMPLES_SHIPPED</t>
-  </si>
-  <si>
-    <t>NUM_OF_SAMPLES_GOOD</t>
-  </si>
-  <si>
-    <t>NUM_OF_PATH_REPORT</t>
-  </si>
-  <si>
-    <t>SHIP_FROM</t>
-  </si>
-  <si>
-    <t>SHIP_TO</t>
+    <t>TRACKING NUMBER</t>
+  </si>
+  <si>
+    <t>ACCOUNT NUMBER</t>
+  </si>
+  <si>
+    <t>SHIPPING CONDITION</t>
+  </si>
+  <si>
+    <t>DATE SHIPPED</t>
+  </si>
+  <si>
+    <t>NUM OF SAMPLES SHIPPED</t>
+  </si>
+  <si>
+    <t>NUM OF SAMPLES GOOD</t>
+  </si>
+  <si>
+    <t>NUM OF PATH REPORT</t>
+  </si>
+  <si>
+    <t>SHIP FROM</t>
+  </si>
+  <si>
+    <t>SHIP TO</t>
   </si>
   <si>
     <t>Filled by Biorepository</t>
@@ -692,133 +692,154 @@
     <t>#d</t>
   </si>
   <si>
-    <t>TRIAL_PARTICIPANT_ID</t>
-  </si>
-  <si>
-    <t>CIMAC_PARTICIPANT_ID</t>
-  </si>
-  <si>
-    <t>COHORT_ID</t>
-  </si>
-  <si>
-    <t>ARM_ID</t>
-  </si>
-  <si>
-    <t>SITE_SAMPLE_ID</t>
-  </si>
-  <si>
-    <t>CIMAC_SAMPLE_ID</t>
-  </si>
-  <si>
-    <t>TIME_POINT</t>
-  </si>
-  <si>
-    <t>BLOOD_COLLECTION_DATE</t>
-  </si>
-  <si>
-    <t>BLOOD_COLLECTION_TIME</t>
-  </si>
-  <si>
-    <t>BLOOD_PROCESSING_DATE</t>
-  </si>
-  <si>
-    <t>BLOOD_PROCESSING_TIME</t>
-  </si>
-  <si>
-    <t>SAMPLE_LOCATION</t>
-  </si>
-  <si>
-    <t>SPECIMEN_TYPE</t>
-  </si>
-  <si>
-    <t>SPECIMEN_FORMAT</t>
+    <t>CIMAC ALIQUOT ID</t>
+  </si>
+  <si>
+    <t>PBMC RECOVERED</t>
+  </si>
+  <si>
+    <t>MATERIAL USED</t>
+  </si>
+  <si>
+    <t>MATERIAL REMAINING</t>
+  </si>
+  <si>
+    <t>SAMPLE QUALITY STATUS</t>
+  </si>
+  <si>
+    <t>SAMPLE REPLACEMENT</t>
+  </si>
+  <si>
+    <t>SAMPLE STATUS</t>
+  </si>
+  <si>
+    <t>TRIAL PARTICIPANT ID</t>
+  </si>
+  <si>
+    <t>CIMAC PARTICIPANT ID</t>
+  </si>
+  <si>
+    <t>COHORT ID</t>
+  </si>
+  <si>
+    <t>ARM ID</t>
+  </si>
+  <si>
+    <t>SITE SAMPLE ID</t>
+  </si>
+  <si>
+    <t>CIMAC SAMPLE ID</t>
+  </si>
+  <si>
+    <t>TIME POINT</t>
+  </si>
+  <si>
+    <t>BLOOD COLLECTION DATE</t>
+  </si>
+  <si>
+    <t>BLOOD COLLECTION TIME</t>
+  </si>
+  <si>
+    <t>BLOOD PROCESSING DATE</t>
+  </si>
+  <si>
+    <t>BLOOD PROCESSING TIME</t>
+  </si>
+  <si>
+    <t>SAMPLE LOCATION</t>
+  </si>
+  <si>
+    <t>SPECIMEN TYPE</t>
+  </si>
+  <si>
+    <t>SPECIMEN FORMAT</t>
   </si>
   <si>
     <t>QUANTITY</t>
   </si>
   <si>
-    <t>VOLUME_QUANTITY</t>
-  </si>
-  <si>
-    <t>VOLUME_UNITS</t>
-  </si>
-  <si>
-    <t>PBMC_ALIQUOTED</t>
-  </si>
-  <si>
-    <t>SAMPLE_SOURCE</t>
-  </si>
-  <si>
-    <t>CIMAC_ALIQUOT_ID</t>
-  </si>
-  <si>
-    <t>PBMC_RECOVERED</t>
-  </si>
-  <si>
-    <t>MATERIAL_USED</t>
-  </si>
-  <si>
-    <t>MATERIAL_REMAINING</t>
-  </si>
-  <si>
-    <t>SAMPLE_QUALITY_STATUS</t>
-  </si>
-  <si>
-    <t>SAMPLE_REPLACEMENT</t>
-  </si>
-  <si>
-    <t>SAMPLE_STATUS</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>e</t>
+    <t>VOLUME QUANTITY</t>
+  </si>
+  <si>
+    <t>VOLUME UNITS</t>
+  </si>
+  <si>
+    <t>PBMC ALIQUOTED</t>
+  </si>
+  <si>
+    <t>SAMPLE SOURCE</t>
+  </si>
+  <si>
+    <t>R123</t>
+  </si>
+  <si>
+    <t>Assay-5</t>
   </si>
   <si>
     <t>USPS</t>
   </si>
   <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>sdsfd</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>dfgd</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>T12098</t>
+  </si>
+  <si>
+    <t>A109123</t>
+  </si>
+  <si>
+    <t>Ambient (Ice Pack)</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>Usable for Assay</t>
+  </si>
+  <si>
+    <t>Replacement Tested</t>
   </si>
   <si>
     <t>Sample Exhausted</t>
   </si>
   <si>
-    <t>Assay-5</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Verifying</t>
-  </si>
-  <si>
-    <t>FFPE Core Punch</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>PBMC</t>
+  </si>
+  <si>
+    <t>EDTA Tube</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>FFPE block #52</t>
+  </si>
+  <si>
+    <t>CIMAC-12345</t>
+  </si>
+  <si>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
+  </si>
+  <si>
+    <t>CIMAC-14345</t>
+  </si>
+  <si>
+    <t>blah blah blah</t>
+  </si>
+  <si>
+    <t>FFPE Scroll</t>
   </si>
 </sst>
 </file>
@@ -929,8 +950,8 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1274,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1305,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1318,15 +1339,15 @@
       <c r="AA1" s="6"/>
       <c r="AB1" s="6"/>
     </row>
-    <row r="2" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
+      <c r="C2" s="1">
+        <v>12345</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1354,15 +1375,15 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
+      <c r="C3" s="1">
+        <v>54321</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1390,7 +1411,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1434,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1469,9 +1490,7 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1506,7 +1525,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1534,7 +1553,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1542,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1570,16 +1589,14 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1606,7 +1623,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1614,7 +1631,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1642,15 +1659,15 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
-        <v>4</v>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1678,15 +1695,15 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1714,15 +1731,15 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>58</v>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1750,7 +1767,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1758,7 +1775,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="3">
-        <v>41071</v>
+        <v>41590</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1786,7 +1803,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1794,7 +1811,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1822,16 +1839,14 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1">
-        <v>7</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1858,7 +1873,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1894,7 +1909,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1930,7 +1945,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1938,7 +1953,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2004,28 +2019,28 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>32</v>
@@ -2090,110 +2105,515 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>123</v>
+      </c>
+      <c r="D23">
+        <v>122</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23">
+        <v>12345</v>
+      </c>
+      <c r="J23">
+        <v>54321</v>
+      </c>
+      <c r="K23">
+        <v>12345</v>
+      </c>
+      <c r="L23">
+        <v>54321</v>
+      </c>
+      <c r="M23">
+        <v>12345</v>
+      </c>
+      <c r="N23">
+        <v>54321</v>
+      </c>
+      <c r="O23">
+        <v>12345</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>41193</v>
+      </c>
+      <c r="R23" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="S23" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T23" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U23" t="s">
+        <v>62</v>
+      </c>
+      <c r="V23" t="s">
+        <v>73</v>
+      </c>
+      <c r="W23" t="s">
+        <v>74</v>
+      </c>
+      <c r="X23">
+        <v>100</v>
+      </c>
+      <c r="Y23">
+        <v>100</v>
+      </c>
+      <c r="Z23" t="s">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J23" s="4">
-        <v>41255</v>
-      </c>
-      <c r="K23" t="s">
-        <v>58</v>
-      </c>
-      <c r="L23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0.42372685185185183</v>
-      </c>
-      <c r="N23" t="s">
-        <v>60</v>
-      </c>
-      <c r="O23" t="s">
-        <v>58</v>
-      </c>
-      <c r="P23" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q23">
-        <v>5</v>
-      </c>
-      <c r="R23">
-        <v>6</v>
-      </c>
-      <c r="S23">
-        <v>6</v>
-      </c>
-      <c r="T23">
-        <v>6</v>
-      </c>
-      <c r="U23">
+      <c r="AA23">
+        <v>10</v>
+      </c>
+      <c r="AB23" t="s">
         <v>66</v>
-      </c>
-      <c r="V23" t="s">
-        <v>61</v>
-      </c>
-      <c r="W23">
-        <v>12364</v>
-      </c>
-      <c r="X23">
-        <v>123456</v>
-      </c>
-      <c r="Y23">
-        <v>1</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>123</v>
+      </c>
+      <c r="D24">
+        <v>122</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I24">
+        <v>12345</v>
+      </c>
+      <c r="J24">
+        <v>54321</v>
+      </c>
+      <c r="K24">
+        <v>12345</v>
+      </c>
+      <c r="L24">
+        <v>54321</v>
+      </c>
+      <c r="M24">
+        <v>12345</v>
+      </c>
+      <c r="N24">
+        <v>54321</v>
+      </c>
+      <c r="O24">
+        <v>12345</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>59</v>
+      </c>
+      <c r="R24" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="S24" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T24" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U24" t="s">
+        <v>62</v>
+      </c>
+      <c r="V24" t="s">
+        <v>63</v>
+      </c>
+      <c r="W24" t="s">
+        <v>64</v>
+      </c>
+      <c r="X24">
+        <v>100</v>
+      </c>
+      <c r="Y24">
+        <v>100</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA24">
+        <v>10</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>123</v>
+      </c>
+      <c r="D25">
+        <v>122</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25">
+        <v>12345</v>
+      </c>
+      <c r="J25">
+        <v>54321</v>
+      </c>
+      <c r="K25">
+        <v>12345</v>
+      </c>
+      <c r="L25">
+        <v>54321</v>
+      </c>
+      <c r="M25">
+        <v>12345</v>
+      </c>
+      <c r="N25">
+        <v>54321</v>
+      </c>
+      <c r="O25">
+        <v>12345</v>
+      </c>
+      <c r="P25" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>41193</v>
+      </c>
+      <c r="R25" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="S25" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T25" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U25" t="s">
+        <v>62</v>
+      </c>
+      <c r="V25" t="s">
+        <v>63</v>
+      </c>
+      <c r="W25" t="s">
+        <v>64</v>
+      </c>
+      <c r="X25">
+        <v>100</v>
+      </c>
+      <c r="Y25">
+        <v>100</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA25">
+        <v>10</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>123</v>
+      </c>
+      <c r="D26">
+        <v>122</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26">
+        <v>12345</v>
+      </c>
+      <c r="J26">
+        <v>54321</v>
+      </c>
+      <c r="K26">
+        <v>12345</v>
+      </c>
+      <c r="L26">
+        <v>54321</v>
+      </c>
+      <c r="M26">
+        <v>12345</v>
+      </c>
+      <c r="N26">
+        <v>54321</v>
+      </c>
+      <c r="O26">
+        <v>12345</v>
+      </c>
+      <c r="P26" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>41193</v>
+      </c>
+      <c r="R26" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="S26" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T26" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U26" t="s">
+        <v>62</v>
+      </c>
+      <c r="V26" t="s">
+        <v>63</v>
+      </c>
+      <c r="W26" t="s">
+        <v>64</v>
+      </c>
+      <c r="X26">
+        <v>100</v>
+      </c>
+      <c r="Y26">
+        <v>100</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA26">
+        <v>10</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>123</v>
+      </c>
+      <c r="D27">
+        <v>122</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27">
+        <v>12345</v>
+      </c>
+      <c r="J27">
+        <v>54321</v>
+      </c>
+      <c r="K27">
+        <v>12345</v>
+      </c>
+      <c r="L27">
+        <v>54321</v>
+      </c>
+      <c r="M27">
+        <v>12345</v>
+      </c>
+      <c r="N27">
+        <v>54321</v>
+      </c>
+      <c r="O27">
+        <v>12345</v>
+      </c>
+      <c r="P27" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>41193</v>
+      </c>
+      <c r="R27" t="s">
+        <v>72</v>
+      </c>
+      <c r="S27" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T27" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U27" t="s">
+        <v>62</v>
+      </c>
+      <c r="V27" t="s">
+        <v>63</v>
+      </c>
+      <c r="W27" t="s">
+        <v>64</v>
+      </c>
+      <c r="X27">
+        <v>100</v>
+      </c>
+      <c r="Y27">
+        <v>100</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA27">
+        <v>10</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28">
+        <v>123</v>
+      </c>
+      <c r="D28">
+        <v>122</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28">
+        <v>12345</v>
+      </c>
+      <c r="J28">
+        <v>54321</v>
+      </c>
+      <c r="K28">
+        <v>12345</v>
+      </c>
+      <c r="L28">
+        <v>54321</v>
+      </c>
+      <c r="M28">
+        <v>12345</v>
+      </c>
+      <c r="N28">
+        <v>54321</v>
+      </c>
+      <c r="O28">
+        <v>12345</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>41193</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="S28" s="5">
+        <v>41193</v>
+      </c>
+      <c r="T28" s="4">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="U28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V28" t="s">
+        <v>63</v>
+      </c>
+      <c r="W28" t="s">
+        <v>64</v>
+      </c>
+      <c r="X28">
+        <v>100</v>
+      </c>
+      <c r="Y28">
+        <v>100</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA28">
+        <v>10</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
@@ -3172,36 +3592,39 @@
     <mergeCell ref="B21:U21"/>
     <mergeCell ref="V21:AB21"/>
   </mergeCells>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{04AE32CC-62AA-094D-B8FD-FEBAFE65ACB9}">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{93E6E103-BB92-304F-A404-6C45E9CE6F4A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{C8D0B440-89F3-DA4E-BD1C-B7BDD5F4A303}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J24:J222 L25:L222" xr:uid="{B043FF79-C2A8-324A-808C-0F39A307D0F6}">
-      <formula1>AND(ISNUMBER(J24:J223),LEFT(CELL("format",J24:J223),1)="D")</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:F222 Q24" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K24:K222 M24:M222" xr:uid="{8EEE7776-21EB-1C41-8148-3AF6CF553FA7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:G222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H23:H222" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="S23:S222 Q23 Q25:Q222" xr:uid="{00000000-0002-0000-0000-000007000000}">
+      <formula1>AND(ISNUMBER(Q23:Q222),LEFT(CELL("format",Q23:Q222),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="T23:T222 R23:R26 R28:R222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O24:O222" xr:uid="{31127FE8-3D13-794D-A378-ADF79A508DFC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V24:V222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{BA0C9242-804E-D048-A79A-80C970AE9357}">
-      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{27EC635B-5DCE-5A44-B5EF-B26D7DA0E8B9}">
-      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{1636BA57-6D76-744E-87D9-89CEC6E49589}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P25:P222 P23" xr:uid="{FF7F145C-86AA-B047-AD61-F29440E30791}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W23:W222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Other,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated PBMC template structure
</commit_message>
<xml_diff>
--- a/tests/data/pbmc_invalid.xlsx
+++ b/tests/data/pbmc_invalid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3D7F3BF-636B-F64A-8DA7-81CF9CE8F9A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637487E-2F96-E54A-8F90-F75A07258E25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50780" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="17140" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -82,7 +82,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -164,7 +164,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
+          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
         </r>
       </text>
     </comment>
@@ -177,7 +177,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shippment made.</t>
+          <t>Type of shipment made.</t>
         </r>
       </text>
     </comment>
@@ -268,7 +268,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial Participant Identifier. Example: PT123.</t>
         </r>
       </text>
     </comment>
@@ -281,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial Participant Identifier. Example: PT123.</t>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
         </r>
       </text>
     </comment>
@@ -294,7 +294,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
         </r>
       </text>
     </comment>
@@ -320,7 +320,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
         </r>
       </text>
     </comment>
@@ -333,7 +333,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -346,7 +346,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
         </r>
       </text>
     </comment>
@@ -359,7 +359,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+          <t>Date of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -372,7 +372,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
+          <t>Time of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -385,7 +385,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood collection.</t>
+          <t>Date of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -398,7 +398,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood processing.</t>
+          <t>Time of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -411,7 +411,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood processing.</t>
+          <t>Sample location within the shipping container. Example: A1.</t>
         </r>
       </text>
     </comment>
@@ -424,7 +424,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
+          <t>Type of sample sent.</t>
         </r>
       </text>
     </comment>
@@ -437,7 +437,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of sample sent.</t>
+          <t>The format in which the sample was sent.</t>
         </r>
       </text>
     </comment>
@@ -450,7 +450,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The format in which the sample was sent.</t>
+          <t>Quantity of each aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each sample shipped.</t>
+          <t>Volume of aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -476,7 +476,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of sample shipped.</t>
+          <t>The unit of biological material from this aliquot.</t>
         </r>
       </text>
     </comment>
@@ -489,7 +489,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unit of each sample. Example: ml.</t>
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
         </r>
       </text>
     </comment>
@@ -502,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
         </r>
       </text>
     </comment>
@@ -515,7 +515,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -528,7 +528,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
         </r>
       </text>
     </comment>
@@ -541,7 +541,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
         </r>
       </text>
     </comment>
@@ -554,7 +554,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
+          <t>Receiving site indicates how much material remains after assay use.</t>
         </r>
       </text>
     </comment>
@@ -567,7 +567,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
+          <t>Final status of aliquot after QC and pathology review.</t>
         </r>
       </text>
     </comment>
@@ -580,7 +580,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
+          <t>Status of aliquot if replacement is/was requested.</t>
         </r>
       </text>
     </comment>
@@ -593,20 +593,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of sample if replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
+          <t>Status of aliquot used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -615,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="74">
   <si>
     <t>#t</t>
   </si>
@@ -797,53 +784,53 @@
     <t>A1</t>
   </si>
   <si>
+    <t>blah blah blah</t>
+  </si>
+  <si>
+    <t>EDTA Tube</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>FFPE block #52</t>
+  </si>
+  <si>
+    <t>Usable for Assay</t>
+  </si>
+  <si>
     <t>PBMC</t>
   </si>
   <si>
-    <t>EDTA Tube</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>FFPE block #52</t>
+    <t>CIMAC-14345</t>
   </si>
   <si>
     <t>CIMAC-12345</t>
   </si>
   <si>
-    <t>Usable for Assay</t>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
   </si>
   <si>
     <t>Replacement Tested</t>
   </si>
   <si>
     <t>Sample Exhausted</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
-  </si>
-  <si>
-    <t>blah blah blah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +849,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -938,14 +931,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1284,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB222"/>
+  <dimension ref="A1:AA222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:O28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1296,41 +1289,40 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-    </row>
-    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1364,9 +1356,8 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1400,9 +1391,8 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1436,9 +1426,8 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1472,9 +1461,8 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1506,9 +1494,8 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1542,9 +1529,8 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1578,9 +1564,8 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1612,9 +1597,8 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1648,9 +1632,8 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1684,9 +1667,8 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1720,9 +1702,8 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1756,16 +1737,15 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1792,9 +1772,8 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1828,9 +1807,8 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1864,9 +1842,8 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1900,9 +1877,8 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1936,9 +1912,8 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1972,659 +1947,636 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
+        <v>54321</v>
+      </c>
+      <c r="C23">
         <v>12345</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>54321</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>12345</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>54321</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>12345</v>
       </c>
-      <c r="G23">
-        <v>54321</v>
-      </c>
-      <c r="H23">
-        <v>12345</v>
-      </c>
-      <c r="I23" s="4">
+      <c r="H23" s="5">
         <v>0.42444444444444446</v>
       </c>
+      <c r="I23" s="6">
+        <v>41193</v>
+      </c>
       <c r="J23" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="K23" s="6">
         <v>41193</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="5">
         <v>0.42444444444444446</v>
       </c>
-      <c r="L23" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.42444444444444446</v>
+      <c r="M23" t="s">
+        <v>59</v>
       </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O23" t="s">
-        <v>73</v>
-      </c>
-      <c r="P23" t="s">
         <v>61</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
       </c>
       <c r="Q23">
         <v>100</v>
       </c>
-      <c r="R23">
+      <c r="R23" t="s">
+        <v>62</v>
+      </c>
+      <c r="S23">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" t="s">
+        <v>67</v>
+      </c>
+      <c r="V23">
+        <v>123</v>
+      </c>
+      <c r="W23">
+        <v>122</v>
+      </c>
+      <c r="X23">
         <v>100</v>
       </c>
-      <c r="S23" t="s">
-        <v>62</v>
-      </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="s">
-        <v>63</v>
-      </c>
-      <c r="V23" t="s">
+      <c r="Y23" t="s">
         <v>64</v>
       </c>
-      <c r="W23">
-        <v>123</v>
-      </c>
-      <c r="X23">
-        <v>122</v>
-      </c>
-      <c r="Y23">
+      <c r="Z23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>54321</v>
+      </c>
+      <c r="C24">
+        <v>12345</v>
+      </c>
+      <c r="D24">
+        <v>54321</v>
+      </c>
+      <c r="E24">
+        <v>12345</v>
+      </c>
+      <c r="F24">
+        <v>54321</v>
+      </c>
+      <c r="G24">
+        <v>12345</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="I24" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="K24" s="6">
+        <v>41193</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="M24" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" t="s">
+        <v>65</v>
+      </c>
+      <c r="O24" t="s">
+        <v>61</v>
+      </c>
+      <c r="P24">
         <v>100</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>12345</v>
-      </c>
-      <c r="C24">
-        <v>54321</v>
-      </c>
-      <c r="D24">
-        <v>12345</v>
-      </c>
-      <c r="E24">
-        <v>54321</v>
-      </c>
-      <c r="F24">
-        <v>12345</v>
-      </c>
-      <c r="G24">
-        <v>54321</v>
-      </c>
-      <c r="H24">
-        <v>12345</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L24" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N24" t="s">
-        <v>59</v>
-      </c>
-      <c r="O24" t="s">
-        <v>60</v>
-      </c>
-      <c r="P24" t="s">
-        <v>61</v>
       </c>
       <c r="Q24">
         <v>100</v>
       </c>
-      <c r="R24">
+      <c r="R24" t="s">
+        <v>62</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>63</v>
+      </c>
+      <c r="U24" t="s">
+        <v>68</v>
+      </c>
+      <c r="V24">
+        <v>123</v>
+      </c>
+      <c r="W24">
+        <v>122</v>
+      </c>
+      <c r="X24">
         <v>100</v>
       </c>
-      <c r="S24" t="s">
-        <v>62</v>
-      </c>
-      <c r="T24">
-        <v>10</v>
-      </c>
-      <c r="U24" t="s">
-        <v>63</v>
-      </c>
-      <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24">
-        <v>123</v>
-      </c>
-      <c r="X24">
-        <v>122</v>
-      </c>
-      <c r="Y24">
+      <c r="Y24" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>54321</v>
+      </c>
+      <c r="C25">
+        <v>12345</v>
+      </c>
+      <c r="D25">
+        <v>54321</v>
+      </c>
+      <c r="E25">
+        <v>12345</v>
+      </c>
+      <c r="F25">
+        <v>54321</v>
+      </c>
+      <c r="G25">
+        <v>12345</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="I25" s="6">
+        <v>41193</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="K25" s="6">
+        <v>41193</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="M25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" t="s">
+        <v>65</v>
+      </c>
+      <c r="O25" t="s">
+        <v>61</v>
+      </c>
+      <c r="P25">
         <v>100</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>12345</v>
-      </c>
-      <c r="C25">
-        <v>54321</v>
-      </c>
-      <c r="D25">
-        <v>12345</v>
-      </c>
-      <c r="E25">
-        <v>54321</v>
-      </c>
-      <c r="F25">
-        <v>12345</v>
-      </c>
-      <c r="G25">
-        <v>54321</v>
-      </c>
-      <c r="H25">
-        <v>12345</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J25" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L25" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N25" t="s">
-        <v>59</v>
-      </c>
-      <c r="O25" t="s">
-        <v>60</v>
-      </c>
-      <c r="P25" t="s">
-        <v>61</v>
       </c>
       <c r="Q25">
         <v>100</v>
       </c>
-      <c r="R25">
+      <c r="R25" t="s">
+        <v>62</v>
+      </c>
+      <c r="S25">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" t="s">
+        <v>69</v>
+      </c>
+      <c r="V25">
+        <v>123</v>
+      </c>
+      <c r="W25">
+        <v>122</v>
+      </c>
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="S25" t="s">
-        <v>62</v>
-      </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="s">
-        <v>63</v>
-      </c>
-      <c r="V25" t="s">
-        <v>69</v>
-      </c>
-      <c r="W25">
-        <v>123</v>
-      </c>
-      <c r="X25">
-        <v>122</v>
-      </c>
-      <c r="Y25">
+      <c r="Y25" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>54321</v>
+      </c>
+      <c r="C26">
+        <v>12345</v>
+      </c>
+      <c r="D26">
+        <v>54321</v>
+      </c>
+      <c r="E26">
+        <v>12345</v>
+      </c>
+      <c r="F26">
+        <v>54321</v>
+      </c>
+      <c r="G26">
+        <v>12345</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="I26" s="6">
+        <v>41193</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="K26" s="6">
+        <v>41193</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="M26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" t="s">
+        <v>65</v>
+      </c>
+      <c r="O26" t="s">
+        <v>61</v>
+      </c>
+      <c r="P26">
         <v>100</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>12345</v>
-      </c>
-      <c r="C26">
-        <v>54321</v>
-      </c>
-      <c r="D26">
-        <v>12345</v>
-      </c>
-      <c r="E26">
-        <v>54321</v>
-      </c>
-      <c r="F26">
-        <v>12345</v>
-      </c>
-      <c r="G26">
-        <v>54321</v>
-      </c>
-      <c r="H26">
-        <v>12345</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J26" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L26" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N26" t="s">
-        <v>59</v>
-      </c>
-      <c r="O26" t="s">
-        <v>60</v>
-      </c>
-      <c r="P26" t="s">
-        <v>61</v>
       </c>
       <c r="Q26">
         <v>100</v>
       </c>
-      <c r="R26">
+      <c r="R26" t="s">
+        <v>62</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>63</v>
+      </c>
+      <c r="U26" t="s">
+        <v>70</v>
+      </c>
+      <c r="V26">
+        <v>123</v>
+      </c>
+      <c r="W26">
+        <v>122</v>
+      </c>
+      <c r="X26">
         <v>100</v>
       </c>
-      <c r="S26" t="s">
-        <v>62</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26" t="s">
-        <v>63</v>
-      </c>
-      <c r="V26" t="s">
-        <v>70</v>
-      </c>
-      <c r="W26">
-        <v>123</v>
-      </c>
-      <c r="X26">
-        <v>122</v>
-      </c>
-      <c r="Y26">
+      <c r="Y26" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>54321</v>
+      </c>
+      <c r="C27">
+        <v>12345</v>
+      </c>
+      <c r="D27">
+        <v>54321</v>
+      </c>
+      <c r="E27">
+        <v>12345</v>
+      </c>
+      <c r="F27">
+        <v>54321</v>
+      </c>
+      <c r="G27">
+        <v>12345</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="I27" s="6">
+        <v>41193</v>
+      </c>
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" s="6">
+        <v>41193</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="M27" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O27" t="s">
+        <v>61</v>
+      </c>
+      <c r="P27">
         <v>100</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>12345</v>
-      </c>
-      <c r="C27">
-        <v>54321</v>
-      </c>
-      <c r="D27">
-        <v>12345</v>
-      </c>
-      <c r="E27">
-        <v>54321</v>
-      </c>
-      <c r="F27">
-        <v>12345</v>
-      </c>
-      <c r="G27">
-        <v>54321</v>
-      </c>
-      <c r="H27">
-        <v>12345</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J27" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K27" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N27" t="s">
-        <v>59</v>
-      </c>
-      <c r="O27" t="s">
-        <v>60</v>
-      </c>
-      <c r="P27" t="s">
-        <v>61</v>
       </c>
       <c r="Q27">
         <v>100</v>
       </c>
-      <c r="R27">
+      <c r="R27" t="s">
+        <v>62</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>63</v>
+      </c>
+      <c r="U27" t="s">
+        <v>71</v>
+      </c>
+      <c r="V27">
+        <v>123</v>
+      </c>
+      <c r="W27">
+        <v>122</v>
+      </c>
+      <c r="X27">
         <v>100</v>
       </c>
-      <c r="S27" t="s">
-        <v>62</v>
-      </c>
-      <c r="T27">
-        <v>10</v>
-      </c>
-      <c r="U27" t="s">
-        <v>63</v>
-      </c>
-      <c r="V27" t="s">
-        <v>71</v>
-      </c>
-      <c r="W27">
-        <v>123</v>
-      </c>
-      <c r="X27">
-        <v>122</v>
-      </c>
-      <c r="Y27">
+      <c r="Y27" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>54321</v>
+      </c>
+      <c r="C28">
+        <v>12345</v>
+      </c>
+      <c r="D28">
+        <v>54321</v>
+      </c>
+      <c r="E28">
+        <v>12345</v>
+      </c>
+      <c r="F28">
+        <v>54321</v>
+      </c>
+      <c r="G28">
+        <v>12345</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="I28" s="6">
+        <v>41193</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="K28" s="6">
+        <v>41193</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="M28" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" t="s">
+        <v>65</v>
+      </c>
+      <c r="O28" t="s">
+        <v>61</v>
+      </c>
+      <c r="P28">
         <v>100</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>12345</v>
-      </c>
-      <c r="C28">
-        <v>54321</v>
-      </c>
-      <c r="D28">
-        <v>12345</v>
-      </c>
-      <c r="E28">
-        <v>54321</v>
-      </c>
-      <c r="F28">
-        <v>12345</v>
-      </c>
-      <c r="G28">
-        <v>54321</v>
-      </c>
-      <c r="H28">
-        <v>12345</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J28" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L28" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N28" t="s">
-        <v>59</v>
-      </c>
-      <c r="O28" t="s">
-        <v>60</v>
-      </c>
-      <c r="P28" t="s">
-        <v>61</v>
       </c>
       <c r="Q28">
         <v>100</v>
       </c>
-      <c r="R28">
+      <c r="R28" t="s">
+        <v>62</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>63</v>
+      </c>
+      <c r="U28" t="s">
+        <v>66</v>
+      </c>
+      <c r="V28">
+        <v>123</v>
+      </c>
+      <c r="W28">
+        <v>122</v>
+      </c>
+      <c r="X28">
         <v>100</v>
       </c>
-      <c r="S28" t="s">
-        <v>62</v>
-      </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="U28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="Y28" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z28" t="s">
         <v>72</v>
       </c>
-      <c r="W28">
-        <v>123</v>
-      </c>
-      <c r="X28">
-        <v>122</v>
-      </c>
-      <c r="Y28">
-        <v>100</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>65</v>
-      </c>
       <c r="AA28" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3581,43 +3533,52 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="B1:AA1"/>
     <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AB21"/>
+    <mergeCell ref="V21:AA21"/>
   </mergeCells>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E740EEFD-BA74-6847-9464-C02DCACF9945}">
+  <dataValidations count="14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{67708337-E64C-F848-A01C-0363F8A18453}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF43E531-8BC8-6A4D-A70A-F0BC18081BCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{07CBB894-EFA0-4B47-B62A-4A3A1774B079}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{4C550642-C2DB-FC4B-AC4E-887CEC51F5F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{27D83B2E-5F65-A944-825E-E39CE98A4794}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{50BA3003-5FF9-B345-9EF8-405B6D32D78A}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{B6C7226D-D5A3-B245-BD4E-81ACB06A4B5B}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J25:J222 J23" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K23:K222 I25:I222 I23" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(I23:I222),LEFT(CELL("format",I23:I222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K28:K222 K23:K26" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L23:L222 J28:J222 J23:J26" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O24:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N24:N222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O29:O222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+      <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R29:R222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+      <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I24 Y23:Y222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA29:AA222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O28" xr:uid="{ABA8D256-7B79-CF4D-9787-990CF35EFC3E}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Other,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222 J24" xr:uid="{00000000-0002-0000-0000-00000A000000}">
-      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
-      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA28" xr:uid="{FD04B0EA-2F29-5C44-AE61-8DF153EFFF4C}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>